<commit_message>
TS 3 PP Corrections Sethu - 21/08/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.5 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028FA333-FB90-4158-933A-860DE3D7629B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA103D2B-408D-476C-9A90-5D9EAD47FECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4440,7 +4440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4637,6 +4637,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4921,9 +4924,9 @@
   <dimension ref="A1:V2393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A470" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="N123" sqref="N123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10291,8 +10294,8 @@
         <f t="shared" si="5"/>
         <v>122</v>
       </c>
-      <c r="N123" s="43" t="s">
-        <v>231</v>
+      <c r="N123" s="69" t="s">
+        <v>226</v>
       </c>
       <c r="O123" s="6"/>
       <c r="P123" s="7"/>

</xml_diff>

<commit_message>
TS padam Template 3.5 and 4.1 - 19/10/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.5 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E3FFA8-4733-4265-99DE-2A478DD297DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7345E2-8295-4610-A22B-17956DBC2744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6483" uniqueCount="1401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6483" uniqueCount="1400">
   <si>
     <t>PS</t>
   </si>
@@ -4236,9 +4236,6 @@
   </si>
   <si>
     <t>VIN</t>
-  </si>
-  <si>
-    <t>NRE</t>
   </si>
 </sst>
 </file>
@@ -4900,7 +4897,7 @@
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U941" sqref="U941"/>
+      <selection pane="bottomLeft" activeCell="U1752" sqref="U1752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -39305,7 +39302,7 @@
       <c r="S941" s="7"/>
       <c r="T941" s="7"/>
       <c r="U941" s="7" t="s">
-        <v>1400</v>
+        <v>80</v>
       </c>
       <c r="V941" s="36" t="s">
         <v>1329</v>
@@ -64772,7 +64769,7 @@
         <f t="shared" si="80"/>
         <v>149</v>
       </c>
-      <c r="N1686" s="36" t="s">
+      <c r="N1686" s="49" t="s">
         <v>292</v>
       </c>
       <c r="V1686" s="36" t="s">
@@ -64804,7 +64801,7 @@
         <f t="shared" si="80"/>
         <v>150</v>
       </c>
-      <c r="N1687" s="36" t="s">
+      <c r="N1687" s="49" t="s">
         <v>549</v>
       </c>
       <c r="O1687" s="7"/>
@@ -64842,7 +64839,7 @@
         <f t="shared" si="80"/>
         <v>151</v>
       </c>
-      <c r="N1688" s="36" t="s">
+      <c r="N1688" s="49" t="s">
         <v>320</v>
       </c>
       <c r="O1688" s="6"/>
@@ -65105,7 +65102,7 @@
         <f t="shared" si="80"/>
         <v>159</v>
       </c>
-      <c r="N1696" s="36" t="s">
+      <c r="N1696" s="49" t="s">
         <v>292</v>
       </c>
       <c r="P1696" s="7"/>
@@ -65135,7 +65132,7 @@
         <f t="shared" si="80"/>
         <v>160</v>
       </c>
-      <c r="N1697" s="36" t="s">
+      <c r="N1697" s="49" t="s">
         <v>549</v>
       </c>
       <c r="O1697" s="6"/>
@@ -65171,7 +65168,7 @@
         <f t="shared" si="80"/>
         <v>161</v>
       </c>
-      <c r="N1698" s="36" t="s">
+      <c r="N1698" s="49" t="s">
         <v>320</v>
       </c>
       <c r="V1698" s="36" t="s">
@@ -72504,7 +72501,6 @@
       <c r="V2393" s="36"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:V1791" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
nmv 30 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.5 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9EEED1-C3D5-4438-BB63-9A232D97FA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324081F1-7392-4A91-BF23-FEFC586C6A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4504,7 +4504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4690,6 +4690,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4973,10 +4976,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1791"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1100" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O84" sqref="O84"/>
+      <selection pane="bottomLeft" activeCell="P1109" sqref="P1109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -28036,7 +28039,7 @@
         <f t="shared" si="29"/>
         <v>61</v>
       </c>
-      <c r="N613" s="62" t="s">
+      <c r="N613" s="64" t="s">
         <v>472</v>
       </c>
       <c r="O613" s="6"/>
@@ -45080,7 +45083,7 @@
         <f t="shared" si="53"/>
         <v>82</v>
       </c>
-      <c r="N1108" s="49" t="s">
+      <c r="N1108" s="64" t="s">
         <v>732</v>
       </c>
       <c r="O1108" s="6"/>
@@ -45113,7 +45116,7 @@
         <f t="shared" si="53"/>
         <v>83</v>
       </c>
-      <c r="N1109" s="49" t="s">
+      <c r="N1109" s="64" t="s">
         <v>561</v>
       </c>
       <c r="O1109" s="7"/>
@@ -45146,7 +45149,7 @@
         <f t="shared" si="53"/>
         <v>84</v>
       </c>
-      <c r="N1110" s="36" t="s">
+      <c r="N1110" s="64" t="s">
         <v>733</v>
       </c>
       <c r="O1110" s="6"/>
@@ -45182,7 +45185,7 @@
         <f t="shared" si="53"/>
         <v>85</v>
       </c>
-      <c r="N1111" s="49" t="s">
+      <c r="N1111" s="64" t="s">
         <v>732</v>
       </c>
       <c r="O1111" s="7"/>
@@ -45215,7 +45218,7 @@
         <f t="shared" si="53"/>
         <v>86</v>
       </c>
-      <c r="N1112" s="49" t="s">
+      <c r="N1112" s="64" t="s">
         <v>734</v>
       </c>
       <c r="O1112" s="7"/>

</xml_diff>